<commit_message>
Update BOM and add Pictures
</commit_message>
<xml_diff>
--- a/BOM/Tisch_BOM.xlsx
+++ b/BOM/Tisch_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4df1e100b677fb0f/Dokumente/GitHub/hexagon-desk/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{3D1A52E0-9162-4319-8702-66AE8E8CBD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C63FD04-8B4D-44AE-8B31-16A5035DA57B}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{3D1A52E0-9162-4319-8702-66AE8E8CBD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C72166BA-2A2D-42FA-B253-B5AC3D329942}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="4845" windowWidth="19935" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tischplatte" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Hexagon PCB</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Metallic Pulver</t>
-  </si>
-  <si>
-    <t>Holzeinsätze M6</t>
   </si>
   <si>
     <t>Epoxid Harz 4.5kg</t>
@@ -246,6 +243,15 @@
   </si>
   <si>
     <t>PCBWay</t>
+  </si>
+  <si>
+    <t>Formtrennband</t>
+  </si>
+  <si>
+    <t>Formentrennband für Epoxidharze - Trennmittel I Release Agents (kandydip.de)</t>
+  </si>
+  <si>
+    <t>Holzeinsätze M6 - 10mm</t>
   </si>
 </sst>
 </file>
@@ -388,14 +394,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>561975</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>545278</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -418,7 +424,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3476626" y="10277475"/>
+          <a:off x="3476626" y="10020300"/>
           <a:ext cx="609600" cy="611953"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -431,15 +437,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>596039</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5489</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>495301</xdr:rowOff>
+      <xdr:rowOff>600076</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -462,7 +468,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3476625" y="9715501"/>
+          <a:off x="3495675" y="8848726"/>
           <a:ext cx="596039" cy="495300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -476,13 +482,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>51792</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>581025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -786,11 +792,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,22 +808,22 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -835,7 +841,7 @@
         <v>210</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -849,11 +855,11 @@
         <v>6.97</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D34" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D35" si="0">B3*C3</f>
         <v>6.97</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -871,7 +877,7 @@
         <v>0.4</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -889,7 +895,7 @@
         <v>1.6</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,7 +913,7 @@
         <v>0.2</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -925,7 +931,7 @@
         <v>0.2</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -943,12 +949,12 @@
         <v>1.4</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -961,7 +967,7 @@
         <v>103.5</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -979,7 +985,7 @@
         <v>7.4</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -997,7 +1003,7 @@
         <v>0.34</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1015,7 +1021,7 @@
         <v>1.3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1033,7 +1039,7 @@
         <v>18.7</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,12 +1057,12 @@
         <v>30.5</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1069,81 +1075,84 @@
         <v>59.99</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>8.99</v>
+        <v>6.05</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>8.99</v>
+        <v>6.05</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>0.3</v>
+        <v>8.99</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8.99</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B18">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1">
-        <v>0.16700000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>8.35</v>
+        <v>6</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1">
-        <v>29.99</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>29.99</v>
+        <v>8.35</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1158,61 +1167,58 @@
     </row>
     <row r="21" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>19.95</v>
+        <v>29.99</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>19.95</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>39</v>
+        <v>29.99</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" s="1">
+        <v>19.95</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>19.95</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
         <v>8.99</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>8.99</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23">
-        <v>100</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="H23" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -1225,156 +1231,156 @@
         <v>2</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
         <v>0.04</v>
       </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>20.3</v>
-      </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>20.3</v>
+        <v>0.16</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>0.24</v>
+        <v>20.3</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>20.3</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1">
-        <v>0.09</v>
+        <v>0.24</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>100</v>
       </c>
       <c r="C29" s="1">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>13</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1">
-        <v>4</v>
+        <v>0.11</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0.44</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>0.95</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>5</v>
@@ -1387,12 +1393,12 @@
         <v>4.75</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -1405,51 +1411,70 @@
         <v>4.75</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="36" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="2">
-        <f>SUM(D2:D34)</f>
-        <v>632.05999999999995</v>
+    <row r="37" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f>SUM(D2:D35)</f>
+        <v>637.96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" display="https://de.aliexpress.com/item/33010351631.html?spm=a2g0o.productlist.0.0.20aa5d43MRbAjL&amp;algo_pvid=b394aa2f-d9a7-4d3f-868b-885e9788a41c&amp;algo_exp_id=b394aa2f-d9a7-4d3f-868b-885e9788a41c-1&amp;pdp_ext_f=%7B%22sku_id%22%3A%2267029907304%22%7D&amp;pdp_npi=2%40dis%21EUR%212.52%211.56%21%21%21%21%21%400b0a0ae216693891661324857ed807%2167029907304%21sea&amp;curPageLogUid=GzwlkDd3Wwsp" xr:uid="{D46C2137-B04A-4C93-98A8-82B7078EAC6A}"/>
     <hyperlink ref="H15" r:id="rId2" location="/577-menge-4_5_kg_3_0_kg_a_1_5_kg_b" display="https://kandydip.de/ecom/prestashop/epoxidharz-dipon/3993-epoxyplast-3d-b50-deep-pour-resin-ultra-diamond-clear-anti-uv-epoxidharz-i-epoxy-resin-diponr.html - /577-menge-4_5_kg_3_0_kg_a_1_5_kg_b" xr:uid="{A3649952-58A9-4B48-BA39-7E53F6FA1EAF}"/>
-    <hyperlink ref="H16" r:id="rId3" location="/300-menge-25_gramm" display="https://kandydip.de/ecom/prestashop/dipon-colorshift-pearls/1590-red-firestorm-colorshift-pearl-pigment-colorshifts-diponr-4063636005364.html?search_query=Red+Firestorm+Colorshift&amp;results=4 - /300-menge-25_gramm" xr:uid="{88B3F99F-DDCE-4ED6-9E7D-A1945A46258B}"/>
-    <hyperlink ref="H17" r:id="rId4" display="https://www.amazon.de/gp/product/B07PYP344Y/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{1939479B-7E54-4098-AE1E-19A9C8C8F3F7}"/>
+    <hyperlink ref="H17" r:id="rId3" location="/300-menge-25_gramm" display="https://kandydip.de/ecom/prestashop/dipon-colorshift-pearls/1590-red-firestorm-colorshift-pearl-pigment-colorshifts-diponr-4063636005364.html?search_query=Red+Firestorm+Colorshift&amp;results=4 - /300-menge-25_gramm" xr:uid="{88B3F99F-DDCE-4ED6-9E7D-A1945A46258B}"/>
+    <hyperlink ref="H18" r:id="rId4" display="https://www.amazon.de/gp/product/B07PYP344Y/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{1939479B-7E54-4098-AE1E-19A9C8C8F3F7}"/>
     <hyperlink ref="H9" r:id="rId5" display="https://www.bauhaus.info/leimholzplatten/exclusivholz-leimholzplatte/p/14035174" xr:uid="{3A2892C9-F4D6-45FC-8A34-748538B8FAB0}"/>
     <hyperlink ref="H11" r:id="rId6" display="https://www.reichelt.de/bus-puffer-3-state-2--6-v-dil-14-74hc-125-p3132.html?CCOUNTRY=445&amp;LANGUAGE=de&amp;trstct=pos_0&amp;nbc=1&amp;&amp;r=1" xr:uid="{B1D8CA93-24AB-40AD-9AE1-1A13554780F8}"/>
     <hyperlink ref="H10" r:id="rId7" display="https://www.reichelt.de/i-o-erweiterung-16bit-1-8-5v-seriell-i2c-dip-28-mcp-23017-e-sp-p140074.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{C20C913E-86E1-48C7-A00A-4D75DF53E6F7}"/>
     <hyperlink ref="H13" r:id="rId8" display="https://www.reichelt.de/steckernetzteil-12-w-5-v-2-4-a-stabilisiert-gs15e-1p1j-p161604.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{C011D5AB-607B-4312-B1D3-E18D3EE53066}"/>
-    <hyperlink ref="H24" r:id="rId9" display="https://www.reichelt.de/kupplungs-leergehaeuse-crimptechnik-4-polig-psk-254-4w-p694.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{83F424E2-805A-4A25-A3F6-4F6299D6CD08}"/>
-    <hyperlink ref="H25" r:id="rId10" display="https://www.reichelt.de/kupplungs-leergehaeuse-crimptechnik-8-polig-psk-254-8w-p14860.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{DA339188-401B-401F-A66D-F82B9187C952}"/>
-    <hyperlink ref="H23" r:id="rId11" display="https://www.reichelt.de/kupplungs-leergehaeuse-crimptechnik-3-polig-psk-254-3w-p14858.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{8FF8E0E3-5688-4B8A-A867-B906FC14691A}"/>
-    <hyperlink ref="H21" r:id="rId12" display="https://www.amazon.de/CLOU-304843-Clou-Hart%C3%B6l-farblos/dp/B004GTYPFC/ref=sr_1_6?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=25H02QFXMQGX&amp;keywords=hart%C3%B6l&amp;qid=1669390770&amp;sprefix=hart%C3%B6l%2Caps%2C136&amp;sr=8-6" xr:uid="{D9A424DF-5EE2-4114-A536-0E7ECC55C888}"/>
-    <hyperlink ref="H26" r:id="rId13" display="https://www.reichelt.de/crimpzange-psk-kontakte-crimpzange-psk-p6844.html?&amp;trstct=pos_1&amp;nbc=1" xr:uid="{E2D82385-29B8-4C38-98AD-D984A686082C}"/>
-    <hyperlink ref="H27" r:id="rId14" display="https://www.reichelt.de/crimpkontakte-fuer-psk-254--20-stueck-psk-kontakte-p14861.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{34CFC417-A9E6-4B79-9601-047A0DC0E497}"/>
-    <hyperlink ref="H28" r:id="rId15" display="https://www.reichelt.de/printstecker-einzelstecker-gewinkelt-3-polig-pss-254-3w-p14910.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{69746ED8-01C1-4A93-9759-004E8603FB84}"/>
-    <hyperlink ref="H29" r:id="rId16" display="https://www.reichelt.de/printstecker-einzelstecker-gewinkelt-4-polig-pss-254-4w-p137974.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{A4E8A772-93AB-42B0-AAF2-1E739407C4E6}"/>
-    <hyperlink ref="H30" r:id="rId17" display="https://www.reichelt.de/printstecker-einzelstecker-gewinkelt-8-polig-pss-254-8w-p14914.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{D2A1C5DC-C175-467A-B0E8-F02D37F8EEE9}"/>
-    <hyperlink ref="H31" r:id="rId18" display="https://www.reichelt.de/raspberry-pi-pico-rp2040-cortex-m0-microusb-rasp-pi-pico-p295706.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{F4DE6D14-63EA-42C2-87BF-4738D0B2080F}"/>
-    <hyperlink ref="H32" r:id="rId19" display="https://www.reichelt.de/kupferlitze-isoliert-10-m-1-x-0-14-mm-blau-litze-bl-p10292.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{FEEEFF93-65B7-4D48-853A-4F00035F0C52}"/>
-    <hyperlink ref="H33" r:id="rId20" display="https://www.reichelt.de/kupferlitze-isoliert-10-m-1-x-0-14-mm-schwarz-litze-sw-p10298.html?search=LITZE+sw" xr:uid="{AF387DB8-AC97-4729-88C8-AF49517BE591}"/>
-    <hyperlink ref="H34" r:id="rId21" display="https://www.reichelt.de/kupferlitze-isoliert-10-m-1-x-0-14-mm-rot-litze-rt-p10297.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{672BD648-7A48-47A3-8625-D4DF05EDB3AD}"/>
-    <hyperlink ref="H22" r:id="rId22" display="https://www.amazon.de/gp/product/B08HQW9PS8/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{92228054-2FCF-43BD-BEE9-9F06F47CC222}"/>
-    <hyperlink ref="H18" r:id="rId23" display="https://www.ebay.de/itm/162277039480" xr:uid="{CAEADB49-5DFA-4FD6-88C1-1A34B7AFE86F}"/>
+    <hyperlink ref="H25" r:id="rId9" display="https://www.reichelt.de/kupplungs-leergehaeuse-crimptechnik-4-polig-psk-254-4w-p694.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{83F424E2-805A-4A25-A3F6-4F6299D6CD08}"/>
+    <hyperlink ref="H26" r:id="rId10" display="https://www.reichelt.de/kupplungs-leergehaeuse-crimptechnik-8-polig-psk-254-8w-p14860.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{DA339188-401B-401F-A66D-F82B9187C952}"/>
+    <hyperlink ref="H24" r:id="rId11" display="https://www.reichelt.de/kupplungs-leergehaeuse-crimptechnik-3-polig-psk-254-3w-p14858.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{8FF8E0E3-5688-4B8A-A867-B906FC14691A}"/>
+    <hyperlink ref="H22" r:id="rId12" display="https://www.amazon.de/CLOU-304843-Clou-Hart%C3%B6l-farblos/dp/B004GTYPFC/ref=sr_1_6?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=25H02QFXMQGX&amp;keywords=hart%C3%B6l&amp;qid=1669390770&amp;sprefix=hart%C3%B6l%2Caps%2C136&amp;sr=8-6" xr:uid="{D9A424DF-5EE2-4114-A536-0E7ECC55C888}"/>
+    <hyperlink ref="H27" r:id="rId13" display="https://www.reichelt.de/crimpzange-psk-kontakte-crimpzange-psk-p6844.html?&amp;trstct=pos_1&amp;nbc=1" xr:uid="{E2D82385-29B8-4C38-98AD-D984A686082C}"/>
+    <hyperlink ref="H28" r:id="rId14" display="https://www.reichelt.de/crimpkontakte-fuer-psk-254--20-stueck-psk-kontakte-p14861.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{34CFC417-A9E6-4B79-9601-047A0DC0E497}"/>
+    <hyperlink ref="H29" r:id="rId15" display="https://www.reichelt.de/printstecker-einzelstecker-gewinkelt-3-polig-pss-254-3w-p14910.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{69746ED8-01C1-4A93-9759-004E8603FB84}"/>
+    <hyperlink ref="H30" r:id="rId16" display="https://www.reichelt.de/printstecker-einzelstecker-gewinkelt-4-polig-pss-254-4w-p137974.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{A4E8A772-93AB-42B0-AAF2-1E739407C4E6}"/>
+    <hyperlink ref="H31" r:id="rId17" display="https://www.reichelt.de/printstecker-einzelstecker-gewinkelt-8-polig-pss-254-8w-p14914.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{D2A1C5DC-C175-467A-B0E8-F02D37F8EEE9}"/>
+    <hyperlink ref="H32" r:id="rId18" display="https://www.reichelt.de/raspberry-pi-pico-rp2040-cortex-m0-microusb-rasp-pi-pico-p295706.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{F4DE6D14-63EA-42C2-87BF-4738D0B2080F}"/>
+    <hyperlink ref="H33" r:id="rId19" display="https://www.reichelt.de/kupferlitze-isoliert-10-m-1-x-0-14-mm-blau-litze-bl-p10292.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{FEEEFF93-65B7-4D48-853A-4F00035F0C52}"/>
+    <hyperlink ref="H34" r:id="rId20" display="https://www.reichelt.de/kupferlitze-isoliert-10-m-1-x-0-14-mm-schwarz-litze-sw-p10298.html?search=LITZE+sw" xr:uid="{AF387DB8-AC97-4729-88C8-AF49517BE591}"/>
+    <hyperlink ref="H35" r:id="rId21" display="https://www.reichelt.de/kupferlitze-isoliert-10-m-1-x-0-14-mm-rot-litze-rt-p10297.html?&amp;trstct=pos_0&amp;nbc=1" xr:uid="{672BD648-7A48-47A3-8625-D4DF05EDB3AD}"/>
+    <hyperlink ref="H23" r:id="rId22" display="https://www.amazon.de/gp/product/B08HQW9PS8/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{92228054-2FCF-43BD-BEE9-9F06F47CC222}"/>
+    <hyperlink ref="H19" r:id="rId23" display="https://www.ebay.de/itm/162277039480" xr:uid="{CAEADB49-5DFA-4FD6-88C1-1A34B7AFE86F}"/>
     <hyperlink ref="H12" r:id="rId24" display="https://www.amazon.de/gp/product/B089DXQDS9/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{B07359EA-8633-4885-A709-66D345D90800}"/>
     <hyperlink ref="H8" r:id="rId25" display="https://www.amazon.de/Aerzetix-Kondensator-chemischen-1500%CE%BCF-%C3%9812-5x20mm/dp/B01N15CYYA/ref=sr_1_7?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=2SZTNTF59O6S3&amp;keywords=kondensator+1500&amp;qid=1669391351&amp;sprefix=kondensator+1500%2Caps%2C77&amp;sr=8-7" xr:uid="{70FC5787-8486-4601-B2DC-3F70F53F4C2F}"/>
     <hyperlink ref="H6" r:id="rId26" display="https://www.amazon.de/gp/product/B07BFMXHN8/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{209F4438-34B0-4B0B-9930-9C5D714975E7}"/>
     <hyperlink ref="H7" r:id="rId27" display="https://www.amazon.de/gp/product/B07TF68QZC/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{12277A0D-C303-4C37-A986-02649E7208B1}"/>
     <hyperlink ref="H4" r:id="rId28" display="https://www.reichelt.de/loetbare-schraubklemme-2-pol-rm-5-mm-90--ctb0102-2-p292680.html?&amp;trstct=pos_1&amp;nbc=1" xr:uid="{953C97BF-75F2-4D72-A916-7DA2485C6DA8}"/>
     <hyperlink ref="H5" r:id="rId29" display="https://www.reichelt.de/loetbare-schraubklemme-3-pol-rm-5-mm-90--ctb0102-3-p292681.html?&amp;trstct=vrt_pdn&amp;nbc=1" xr:uid="{A514B994-08D3-4CB4-A067-3B37A5058413}"/>
+    <hyperlink ref="H16" r:id="rId30" display="https://kandydip.de/ecom/prestashop/trennmittel-i-release-agents/4010-formentrennband-fur-epoxidharze-trennmittel-i-release-agents-diponr-4063636027441.html" xr:uid="{F6BD0F22-2251-4F52-BAB2-24F88D111087}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId30"/>
-  <drawing r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId31"/>
+  <drawing r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>